<commit_message>
some changes for report in github
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Density" sheetId="1" r:id="rId1"/>
@@ -684,20 +684,20 @@
   <dimension ref="B1:O21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
@@ -711,7 +711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -725,7 +725,7 @@
         <v>30.07</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -739,7 +739,7 @@
         <v>28.053999999999998</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -753,7 +753,7 @@
         <v>31.998000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -768,7 +768,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -809,7 +809,7 @@
       <c r="N8" s="7"/>
       <c r="O8" s="8"/>
     </row>
-    <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G9" s="9" t="s">
         <v>11</v>
       </c>
@@ -822,7 +822,7 @@
       <c r="N9" s="10"/>
       <c r="O9" s="11"/>
     </row>
-    <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G10" s="9" t="s">
         <v>17</v>
       </c>
@@ -835,41 +835,41 @@
       <c r="N10" s="10"/>
       <c r="O10" s="11"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I14" s="1"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I16" s="2"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I17" s="1"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I18" s="2"/>
     </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I21" s="2"/>
     </row>
   </sheetData>
@@ -886,19 +886,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R12"/>
+  <dimension ref="B1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
@@ -918,7 +919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -938,7 +939,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -958,7 +959,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -978,7 +979,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -998,7 +999,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1018,7 +1019,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1038,8 +1039,20 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <f>D3*10^-3</f>
+        <v>1.9225000000000003E-2</v>
+      </c>
+      <c r="E10">
+        <f>E3*10^-6</f>
+        <v>-5.5609999999999998E-6</v>
+      </c>
+      <c r="F10">
+        <f>F3*10^5</f>
+        <v>0</v>
+      </c>
       <c r="J10" s="6" t="s">
         <v>10</v>
       </c>
@@ -1052,7 +1065,19 @@
       <c r="Q10" s="7"/>
       <c r="R10" s="8"/>
     </row>
-    <row r="11" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <f t="shared" ref="D11:D15" si="0">D4*10^-3</f>
+        <v>1.4394000000000001E-2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:E15" si="1">E4*10^-6</f>
+        <v>-4.3920000000000005E-6</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:F15" si="2">F4*10^5</f>
+        <v>0</v>
+      </c>
       <c r="J11" s="9" t="s">
         <v>19</v>
       </c>
@@ -1065,7 +1090,19 @@
       <c r="Q11" s="10"/>
       <c r="R11" s="11"/>
     </row>
-    <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>5.0600000000000005E-4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>-22700</v>
+      </c>
       <c r="J12" s="9" t="s">
         <v>18</v>
       </c>
@@ -1077,6 +1114,48 @@
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="11"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1.0449999999999999E-3</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>-115700</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>5.5700000000000009E-4</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>-3100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1.4499999999999999E-3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>12100</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Not important update N2 coeffient
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135"/>
   </bookViews>
   <sheets>
     <sheet name="Density" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>C2H6</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>چون فشار 1atm هست، Pr خیلی کوچک می شود و فرض ایده آلی درست است.</t>
+  </si>
+  <si>
+    <t>N2</t>
   </si>
 </sst>
 </file>
@@ -114,7 +117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,8 +135,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -208,13 +217,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -222,15 +301,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -248,6 +324,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -255,7 +355,303 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -392,6 +788,34 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Component_prop" displayName="Component_prop" ref="B2:E9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5" headerRowCellStyle="Heading 4">
+  <autoFilter ref="B2:E9"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Component" dataDxfId="4" dataCellStyle="Heading 4"/>
+    <tableColumn id="2" name="Tc(K)" dataDxfId="3" dataCellStyle="Output"/>
+    <tableColumn id="3" name="Pc(Pa)" dataDxfId="2" dataCellStyle="Output"/>
+    <tableColumn id="4" name="Mw" dataDxfId="1" dataCellStyle="Output"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Cp" displayName="Cp" ref="B2:G9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16" headerRowCellStyle="Heading 4" dataCellStyle="Output">
+  <autoFilter ref="B2:G9"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Component" dataDxfId="15" dataCellStyle="Heading 4"/>
+    <tableColumn id="2" name="A" dataDxfId="14" dataCellStyle="Output"/>
+    <tableColumn id="3" name="10^3*B" dataDxfId="13" dataCellStyle="Output"/>
+    <tableColumn id="4" name="10^6*C" dataDxfId="12" dataCellStyle="Output"/>
+    <tableColumn id="5" name="10^-5*D" dataDxfId="11" dataCellStyle="Output"/>
+    <tableColumn id="6" name="Tmax" dataDxfId="10" dataCellStyle="Output"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -681,159 +1105,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O21"/>
+  <dimension ref="B2:O21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>305.40600000000001</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>4880109.3</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>30.07</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>282.34379999999999</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>5045426.8</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>28.053999999999998</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>154.64500000000001</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>5043212.7</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>31.998000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>304.15480000000002</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>7380861.7999999998</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>44.009</v>
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>134.18</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>3710045.7</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>28.01</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="16">
         <v>647.10810000000004</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="16">
         <v>22072227.399999999</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="17">
         <v>18.015000000000001</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="8"/>
-    </row>
-    <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G9" s="9" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="7"/>
+    </row>
+    <row r="9" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="16">
+        <v>126.2069</v>
+      </c>
+      <c r="D9" s="16">
+        <v>3398154.1</v>
+      </c>
+      <c r="E9" s="16">
+        <v>28.013999999999999</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="11"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="10"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="11"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="10"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I11" s="2"/>
@@ -881,203 +1316,226 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R12"/>
+  <dimension ref="B2:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:G15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>1.131</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>19.225000000000001</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>-5.5609999999999999</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>1500</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>1.4239999999999999</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>14.394</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>-4.3920000000000003</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>1500</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>3.6389999999999998</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>0.50600000000000001</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>-0.22700000000000001</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>2000</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>5.4569999999999999</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>1.0449999999999999</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>0</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>-1.157</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>2000</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>3.3759999999999999</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>0.55700000000000005</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>0</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>-3.1E-2</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>2500</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="16">
         <v>3.47</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="16">
         <v>1.45</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="16">
         <v>0</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="16">
         <v>0.121</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="17">
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="16">
+        <v>3.28</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0.04</v>
+      </c>
+      <c r="G9" s="17">
+        <v>2000</v>
+      </c>
+    </row>
     <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="8"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="7"/>
     </row>
     <row r="11" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="11"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="10"/>
     </row>
     <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="11"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1088,5 +1546,8 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
write the gas phase balance
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9132" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Density" sheetId="1" r:id="rId1"/>
@@ -1120,19 +1120,19 @@
   <dimension ref="B2:O21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>30.07</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>28.053999999999998</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>31.998000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1219,7 +1219,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
@@ -1244,7 +1244,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="15"/>
     </row>
-    <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
         <v>20</v>
       </c>
@@ -1269,7 +1269,7 @@
       <c r="N9" s="17"/>
       <c r="O9" s="18"/>
     </row>
-    <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G10" s="16" t="s">
         <v>17</v>
       </c>
@@ -1282,41 +1282,41 @@
       <c r="N10" s="17"/>
       <c r="O10" s="18"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I14" s="1"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I16" s="2"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I17" s="1"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I18" s="2"/>
     </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I21" s="2"/>
     </row>
   </sheetData>
@@ -1342,15 +1342,15 @@
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
         <v>20</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J10" s="13" t="s">
         <v>10</v>
       </c>
@@ -1523,7 +1523,7 @@
       <c r="Q10" s="14"/>
       <c r="R10" s="15"/>
     </row>
-    <row r="11" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J11" s="16" t="s">
         <v>19</v>
       </c>
@@ -1536,7 +1536,7 @@
       <c r="Q11" s="17"/>
       <c r="R11" s="18"/>
     </row>
-    <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J12" s="16" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
adding of Delta Enthalpy reaction standard data in excel
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Density" sheetId="1" r:id="rId1"/>
     <sheet name="Cp" sheetId="2" r:id="rId2"/>
+    <sheet name="DeltaHstand" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>C2H6</t>
   </si>
@@ -78,13 +79,40 @@
   </si>
   <si>
     <t>N2</t>
+  </si>
+  <si>
+    <t>Reactions</t>
+  </si>
+  <si>
+    <t>Heat of reactions Kj/mol</t>
+  </si>
+  <si>
+    <t>Reaction(1)</t>
+  </si>
+  <si>
+    <t>Reaction(2)</t>
+  </si>
+  <si>
+    <t>Reaction(3)</t>
+  </si>
+  <si>
+    <t>Reaction(4)</t>
+  </si>
+  <si>
+    <t>Reaction(5)</t>
+  </si>
+  <si>
+    <t>https://sci-hub.tw/10.1016/j.cherd.2019.04.028#</t>
+  </si>
+  <si>
+    <t>Ref</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +140,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -288,12 +331,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -331,6 +375,24 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -350,12 +412,32 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Heading 4" xfId="1" builtinId="19"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="22">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -790,8 +872,51 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>418420</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123618</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="552450" y="2486025"/>
+          <a:ext cx="5438095" cy="1657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Component_prop" displayName="Component_prop" ref="B2:E9" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15" headerRowCellStyle="Heading 4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Component_prop" displayName="Component_prop" ref="B2:E9" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18" headerRowCellStyle="Heading 4">
   <autoFilter ref="B2:E9">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -799,17 +924,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Component" dataDxfId="14" dataCellStyle="Heading 4"/>
-    <tableColumn id="2" name="Tc(K)" dataDxfId="13" dataCellStyle="Output"/>
-    <tableColumn id="3" name="Pc(Pa)" dataDxfId="12" dataCellStyle="Output"/>
-    <tableColumn id="4" name="Mw" dataDxfId="11" dataCellStyle="Output"/>
+    <tableColumn id="1" name="Component" dataDxfId="17" dataCellStyle="Heading 4"/>
+    <tableColumn id="2" name="Tc(K)" dataDxfId="16" dataCellStyle="Output"/>
+    <tableColumn id="3" name="Pc(Pa)" dataDxfId="15" dataCellStyle="Output"/>
+    <tableColumn id="4" name="Mw" dataDxfId="14" dataCellStyle="Output"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Cp" displayName="Cp" ref="B2:G9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6" headerRowCellStyle="Heading 4" dataCellStyle="Output">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Cp" displayName="Cp" ref="B2:G9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9" headerRowCellStyle="Heading 4" dataCellStyle="Output">
   <autoFilter ref="B2:G9">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -819,14 +944,28 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="Component" dataDxfId="5" dataCellStyle="Heading 4"/>
-    <tableColumn id="2" name="A" dataDxfId="4" dataCellStyle="Output"/>
-    <tableColumn id="3" name="10^3*B" dataDxfId="3" dataCellStyle="Output"/>
-    <tableColumn id="4" name="10^6*C" dataDxfId="2" dataCellStyle="Output"/>
-    <tableColumn id="5" name="10^-5*D" dataDxfId="1" dataCellStyle="Output"/>
-    <tableColumn id="6" name="Tmax" dataDxfId="0" dataCellStyle="Output"/>
+    <tableColumn id="1" name="Component" dataDxfId="8" dataCellStyle="Heading 4"/>
+    <tableColumn id="2" name="A" dataDxfId="7" dataCellStyle="Output"/>
+    <tableColumn id="3" name="10^3*B" dataDxfId="6" dataCellStyle="Output"/>
+    <tableColumn id="4" name="10^6*C" dataDxfId="5" dataCellStyle="Output"/>
+    <tableColumn id="5" name="10^-5*D" dataDxfId="4" dataCellStyle="Output"/>
+    <tableColumn id="6" name="Tmax" dataDxfId="3" dataCellStyle="Output"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="C4:D10" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="C4:D10">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Reactions" dataDxfId="1"/>
+    <tableColumn id="2" name="Heat of reactions Kj/mol" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1219,7 +1358,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
@@ -1232,17 +1371,17 @@
       <c r="E8" s="11">
         <v>18.015000000000001</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="15"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="21"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
@@ -1257,30 +1396,30 @@
       <c r="E9" s="10">
         <v>28.013999999999999</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="18"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="24"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="18"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="24"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I11" s="2"/>
@@ -1338,7 +1477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
@@ -1511,43 +1650,43 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="15"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="21"/>
     </row>
     <row r="11" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="18"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="24"/>
     </row>
     <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="18"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1562,4 +1701,87 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="13">
+        <v>-111.43</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="13">
+        <v>-1443.15</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="13">
+        <v>-860</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="13">
+        <v>-1331.81</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="13">
+        <v>-760</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>